<commit_message>
Generated new sample expense reports.
</commit_message>
<xml_diff>
--- a/expenses-report.xlsx
+++ b/expenses-report.xlsx
@@ -10,15 +10,117 @@
     <sheet name="DBS Altitude" sheetId="1" r:id="rId1"/>
     <sheet name="CITI Rewards Card" sheetId="2" r:id="rId2"/>
     <sheet name="Standard Charted 1.5% Cashback" sheetId="3" r:id="rId3"/>
+    <sheet name="Debt Collection" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="23">
+  <si>
+    <t>DBS Altitude</t>
+  </si>
+  <si>
+    <t>Billing Cycle:</t>
+  </si>
+  <si>
+    <t>Date</t>
+  </si>
+  <si>
+    <t>12/08/2020 to 11/09/2020</t>
+  </si>
+  <si>
+    <t>Category</t>
+  </si>
+  <si>
+    <t>Food</t>
+  </si>
+  <si>
+    <t>12/09/2020 to 11/10/2020</t>
+  </si>
+  <si>
+    <t>Amount</t>
+  </si>
+  <si>
+    <t>Transaction_Details</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>Payee</t>
+  </si>
+  <si>
+    <t>Kin Zhong</t>
+  </si>
+  <si>
+    <t>Shared</t>
+  </si>
+  <si>
+    <t>Total Amount</t>
+  </si>
+  <si>
+    <t>30</t>
+  </si>
+  <si>
+    <t>31</t>
+  </si>
+  <si>
+    <t>CITI Rewards Card</t>
+  </si>
+  <si>
+    <t>NIL</t>
+  </si>
+  <si>
+    <t>Standard Charted 1.5% Cashback</t>
+  </si>
+  <si>
+    <t>Payment_Method</t>
+  </si>
+  <si>
+    <t>Total Sum:</t>
+  </si>
+  <si>
+    <t>61</t>
+  </si>
+  <si>
+    <t>30.5</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="1">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="dd/mm/yyyy"/>
+  </numFmts>
+  <fonts count="4">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="17"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -34,7 +136,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -42,12 +144,36 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -342,45 +468,615 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+  <dimension ref="A1:H10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="30.7109375" style="1" customWidth="1"/>
+    <col min="1" max="1" width="12.7109375" style="1" customWidth="1"/>
+    <col min="2" max="4" width="20.7109375" style="1" customWidth="1"/>
+    <col min="5" max="5" width="33.7109375" style="1" customWidth="1"/>
+    <col min="6" max="8" width="20.7109375" style="1" customWidth="1"/>
   </cols>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:8">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" s="3" customFormat="1">
+      <c r="A3" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" s="3" customFormat="1">
+      <c r="A4" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="G4" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="H4" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8">
+      <c r="A5" s="4">
+        <v>44055</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C5" s="1">
+        <v>10</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8">
+      <c r="A6" s="4">
+        <v>44085</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C6" s="1">
+        <v>20</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" s="3" customFormat="1">
+      <c r="A8" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" s="3" customFormat="1">
+      <c r="A9" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E9" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="G9" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="H9" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8">
+      <c r="A10" s="4">
+        <v>44086</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C10" s="1">
+        <v>31</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+  <dimension ref="A1:H10"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="30.7109375" style="1" customWidth="1"/>
+    <col min="1" max="1" width="12.7109375" style="1" customWidth="1"/>
+    <col min="2" max="4" width="20.7109375" style="1" customWidth="1"/>
+    <col min="5" max="5" width="33.7109375" style="1" customWidth="1"/>
+    <col min="6" max="8" width="20.7109375" style="1" customWidth="1"/>
   </cols>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:8">
+      <c r="A1" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" s="3" customFormat="1">
+      <c r="A3" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" s="3" customFormat="1">
+      <c r="A4" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="G4" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="H4" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8">
+      <c r="A5" s="4">
+        <v>44055</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C5" s="1">
+        <v>10</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8">
+      <c r="A6" s="4">
+        <v>44085</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C6" s="1">
+        <v>20</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" s="3" customFormat="1">
+      <c r="A8" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" s="3" customFormat="1">
+      <c r="A9" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E9" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="G9" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="H9" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8">
+      <c r="A10" s="4">
+        <v>44087</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C10" s="1">
+        <v>31</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+  <dimension ref="A1:H10"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="30.7109375" style="1" customWidth="1"/>
+    <col min="1" max="1" width="12.7109375" style="1" customWidth="1"/>
+    <col min="2" max="4" width="20.7109375" style="1" customWidth="1"/>
+    <col min="5" max="5" width="33.7109375" style="1" customWidth="1"/>
+    <col min="6" max="8" width="20.7109375" style="1" customWidth="1"/>
   </cols>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:8">
+      <c r="A1" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" s="3" customFormat="1">
+      <c r="A3" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" s="3" customFormat="1">
+      <c r="A4" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="G4" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="H4" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8">
+      <c r="A5" s="4">
+        <v>44055</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C5" s="1">
+        <v>10</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8">
+      <c r="A6" s="4">
+        <v>44085</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C6" s="1">
+        <v>20</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" s="3" customFormat="1">
+      <c r="A8" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" s="3" customFormat="1">
+      <c r="A9" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E9" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="G9" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="H9" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8">
+      <c r="A10" s="4">
+        <v>44087</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C10" s="1">
+        <v>31</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:F13"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="3" width="11.7109375" style="1" customWidth="1"/>
+    <col min="4" max="6" width="23.7109375" style="1" customWidth="1"/>
+    <col min="5" max="5" width="35.7109375" style="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6">
+      <c r="A1" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
+      <c r="A2" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E2" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="F2" s="5" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
+      <c r="A3" s="4">
+        <v>44055</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" s="1">
+        <v>10</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
+      <c r="A4" s="4">
+        <v>44086</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4" s="1">
+        <v>31</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
+      <c r="A5" s="4">
+        <v>44085</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C5" s="1">
+        <v>20</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" s="3" customFormat="1">
+      <c r="A6" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6">
+      <c r="A8" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6">
+      <c r="A9" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="C9" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D9" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E9" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="F9" s="5" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6">
+      <c r="A10" s="4">
+        <v>44085</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C10" s="1">
+        <v>20</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6">
+      <c r="A11" s="4">
+        <v>44055</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C11" s="1">
+        <v>10</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6">
+      <c r="A12" s="4">
+        <v>44087</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C12" s="1">
+        <v>31</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="F12" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" s="3" customFormat="1">
+      <c r="A13" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>22</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>